<commit_message>
27.01.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/27.01.2020 Requisition of Mughdo Corporation.xlsx
+++ b/2020/Requisition/27.01.2020 Requisition of Mughdo Corporation.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\Requisition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D0096-2BB5-412D-850C-A306E922D632}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE48222-10CB-454C-93CE-420C87F23950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="600" windowWidth="16140" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Requisition" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Daily Requisition'!$A$3:$E$95</definedName>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="134">
   <si>
     <t>Model Name</t>
   </si>
@@ -424,21 +423,12 @@
     <t>BL98</t>
   </si>
   <si>
-    <t>SB Tel Enterprises Ltd</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
     <t xml:space="preserve">Blue </t>
   </si>
   <si>
-    <t xml:space="preserve">White &amp; Gold </t>
-  </si>
-  <si>
-    <t>sdaesrtdxhfcjkl.n,jhmvngcbxv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Only White </t>
   </si>
   <si>
@@ -452,6 +442,9 @@
   </si>
   <si>
     <t>27.01.2020</t>
+  </si>
+  <si>
+    <t>Edison Industries Ltd</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1119,10 @@
   <dimension ref="A1:BV108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E104" sqref="E104"/>
+      <selection pane="bottomRight" activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1163,7 +1156,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -1365,17 +1358,19 @@
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B7" s="9">
         <v>760.9</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="8">
+        <v>20</v>
+      </c>
       <c r="D7" s="10">
         <f>C7*B7</f>
-        <v>0</v>
+        <v>15218</v>
       </c>
       <c r="E7" s="40" t="s">
         <v>98</v>
@@ -1450,17 +1445,19 @@
       <c r="BU7" s="26"/>
       <c r="BV7" s="26"/>
     </row>
-    <row r="8" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="9">
         <v>769.92</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="8">
+        <v>30</v>
+      </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23097.599999999999</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>92</v>
@@ -1573,7 +1570,7 @@
     </row>
     <row r="11" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B11" s="9">
         <v>779.96</v>
@@ -1600,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
@@ -1905,14 +1902,14 @@
         <v>1140.845</v>
       </c>
       <c r="C23" s="8">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D23" s="12">
         <f>C23*B23</f>
-        <v>165422.52499999999</v>
+        <v>171126.75</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -2032,17 +2029,19 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:74" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>89</v>
       </c>
       <c r="B27" s="9">
         <v>907.26</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="8">
+        <v>20</v>
+      </c>
       <c r="D27" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18145.2</v>
       </c>
       <c r="E27" s="40" t="s">
         <v>119</v>
@@ -2347,17 +2346,19 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:74" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B34" s="9">
         <v>4885.6000000000004</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="8">
+        <v>10</v>
+      </c>
       <c r="D34" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48856</v>
       </c>
       <c r="E34" s="40" t="s">
         <v>123</v>
@@ -2636,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -3002,19 +3003,17 @@
       </c>
       <c r="E67" s="8"/>
     </row>
-    <row r="68" spans="1:74" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B68" s="9">
         <v>4174.41</v>
       </c>
-      <c r="C68" s="8">
-        <v>5</v>
-      </c>
+      <c r="C68" s="8"/>
       <c r="D68" s="10">
         <f t="shared" si="1"/>
-        <v>20872.05</v>
+        <v>0</v>
       </c>
       <c r="E68" s="40" t="s">
         <v>124</v>
@@ -3085,17 +3084,17 @@
         <v>78</v>
       </c>
       <c r="B73" s="9">
-        <v>4438.07</v>
+        <v>4076.68</v>
       </c>
       <c r="C73" s="8">
         <v>10</v>
       </c>
       <c r="D73" s="10">
         <f t="shared" si="1"/>
-        <v>44380.7</v>
+        <v>40766.799999999996</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="F73" s="32"/>
       <c r="G73" s="32"/>
@@ -3850,7 +3849,7 @@
         <v>0</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F92" s="32"/>
       <c r="G92" s="32"/>
@@ -3916,7 +3915,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:74" ht="15" x14ac:dyDescent="0.25">
@@ -3934,7 +3933,7 @@
         <v>81012.399999999994</v>
       </c>
       <c r="E94" s="40" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="1:74" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -3960,11 +3959,11 @@
       <c r="B96" s="47"/>
       <c r="C96" s="16">
         <f>SUBTOTAL(9,C7:C95)</f>
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="D96" s="17">
         <f>SUBTOTAL(9,D7:D95)</f>
-        <v>311687.67499999993</v>
+        <v>398222.75</v>
       </c>
       <c r="E96" s="31"/>
       <c r="F96" s="33"/>
@@ -4124,7 +4123,7 @@
         <v>350000</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="G101" s="38"/>
       <c r="H101" s="38"/>
@@ -4214,24 +4213,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6D1FFE-B8CB-4799-A112-9572376C5864}">
-  <dimension ref="F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="12" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>